<commit_message>
added new Hungarian alternations sheet
</commit_message>
<xml_diff>
--- a/Combo/Alternations.xlsx
+++ b/Combo/Alternations.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moore-cantwell\GSRs\Combo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF688C11-F0B5-4783-8C57-2AF199AEC721}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB8F5D7-0718-49F0-8742-4C058EB1B534}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11565" xr2:uid="{888022E4-214E-4A4A-BFD9-04B72A4824A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="11565" activeTab="2" xr2:uid="{888022E4-214E-4A4A-BFD9-04B72A4824A8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Voicing_3types" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1969" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="107">
   <si>
     <t>input</t>
   </si>
@@ -251,6 +252,102 @@
   </si>
   <si>
     <t>*voiceFinal</t>
+  </si>
+  <si>
+    <t>domEn_nak</t>
+  </si>
+  <si>
+    <t>domEn_nek</t>
+  </si>
+  <si>
+    <t>bohEm_nVk</t>
+  </si>
+  <si>
+    <t>domEn_nVk</t>
+  </si>
+  <si>
+    <t>bohEm_nak</t>
+  </si>
+  <si>
+    <t>honvEd_nVk</t>
+  </si>
+  <si>
+    <t>poEn_nVk</t>
+  </si>
+  <si>
+    <t>honvEd_nak</t>
+  </si>
+  <si>
+    <t>poEn_nak</t>
+  </si>
+  <si>
+    <t>bohEm_nek</t>
+  </si>
+  <si>
+    <t>honvEd_nek</t>
+  </si>
+  <si>
+    <t>poEn_nek</t>
+  </si>
+  <si>
+    <t>kert_nVk</t>
+  </si>
+  <si>
+    <t>TIm_nVk</t>
+  </si>
+  <si>
+    <t>repes_nVk</t>
+  </si>
+  <si>
+    <t>kert_nak</t>
+  </si>
+  <si>
+    <t>TIm_nak</t>
+  </si>
+  <si>
+    <t>repes_nak</t>
+  </si>
+  <si>
+    <t>kert_nek</t>
+  </si>
+  <si>
+    <t>TIm_nek</t>
+  </si>
+  <si>
+    <t>repes_nek</t>
+  </si>
+  <si>
+    <t>Agree-bk-nonLoc</t>
+  </si>
+  <si>
+    <t>Agree-front-loc</t>
+  </si>
+  <si>
+    <t>Agree-nonhigh-front-loc</t>
+  </si>
+  <si>
+    <t>Agree-low-front-loc</t>
+  </si>
+  <si>
+    <t>B_nVK</t>
+  </si>
+  <si>
+    <t>Bi_nVk</t>
+  </si>
+  <si>
+    <t>BE_nVk</t>
+  </si>
+  <si>
+    <t>Be_nVk</t>
+  </si>
+  <si>
+    <t>BNi_nVk</t>
+  </si>
+  <si>
+    <t>BNE_nVk</t>
+  </si>
+  <si>
+    <t>BNe_nVk</t>
   </si>
 </sst>
 </file>
@@ -1127,13 +1224,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9207142-EE2D-4124-B143-5BB5C7C35764}">
   <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C123" sqref="C123"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -4647,217 +4746,217 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:I21 A22:E61 I22:I61">
-    <cfRule type="expression" dxfId="0" priority="51">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:G21">
-    <cfRule type="expression" dxfId="49" priority="49">
+    <cfRule type="expression" dxfId="48" priority="49">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A82:A121 I62:I121 D82:E121">
-    <cfRule type="expression" dxfId="48" priority="48">
+    <cfRule type="expression" dxfId="47" priority="48">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:E62 A63:A81 C63:E63 B63:B121 D64:E81">
-    <cfRule type="expression" dxfId="47" priority="47">
+    <cfRule type="expression" dxfId="46" priority="47">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22:H41">
-    <cfRule type="expression" dxfId="46" priority="46">
+    <cfRule type="expression" dxfId="45" priority="46">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:G37 F38:F41">
-    <cfRule type="expression" dxfId="45" priority="45">
+    <cfRule type="expression" dxfId="44" priority="45">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42:H61">
-    <cfRule type="expression" dxfId="44" priority="44">
+    <cfRule type="expression" dxfId="43" priority="44">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F42:F61">
-    <cfRule type="expression" dxfId="43" priority="43">
+    <cfRule type="expression" dxfId="42" priority="43">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H62:H81">
-    <cfRule type="expression" dxfId="42" priority="42">
+    <cfRule type="expression" dxfId="41" priority="42">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F62:G81">
-    <cfRule type="expression" dxfId="1" priority="41">
+    <cfRule type="expression" dxfId="40" priority="41">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H82:H101">
-    <cfRule type="expression" dxfId="41" priority="40">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F82:G101">
-    <cfRule type="expression" dxfId="40" priority="39">
+    <cfRule type="expression" dxfId="38" priority="39">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H102:H121">
-    <cfRule type="expression" dxfId="39" priority="38">
+    <cfRule type="expression" dxfId="37" priority="38">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F102:G121">
-    <cfRule type="expression" dxfId="38" priority="37">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:C65">
-    <cfRule type="expression" dxfId="37" priority="36">
+    <cfRule type="expression" dxfId="35" priority="36">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C67">
-    <cfRule type="expression" dxfId="36" priority="35">
+    <cfRule type="expression" dxfId="34" priority="35">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C68:C69">
-    <cfRule type="expression" dxfId="35" priority="34">
+    <cfRule type="expression" dxfId="33" priority="34">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:C71">
-    <cfRule type="expression" dxfId="34" priority="33">
+    <cfRule type="expression" dxfId="32" priority="33">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C73">
-    <cfRule type="expression" dxfId="33" priority="32">
+    <cfRule type="expression" dxfId="31" priority="32">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74:C75">
-    <cfRule type="expression" dxfId="32" priority="31">
+    <cfRule type="expression" dxfId="30" priority="31">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76:C77">
-    <cfRule type="expression" dxfId="31" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C78:C79">
-    <cfRule type="expression" dxfId="30" priority="29">
+    <cfRule type="expression" dxfId="28" priority="29">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C81">
-    <cfRule type="expression" dxfId="29" priority="28">
+    <cfRule type="expression" dxfId="27" priority="28">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:C83">
-    <cfRule type="expression" dxfId="28" priority="27">
+    <cfRule type="expression" dxfId="26" priority="27">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84:C85">
-    <cfRule type="expression" dxfId="27" priority="26">
+    <cfRule type="expression" dxfId="25" priority="26">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:C87">
-    <cfRule type="expression" dxfId="26" priority="25">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:C89">
-    <cfRule type="expression" dxfId="25" priority="24">
+    <cfRule type="expression" dxfId="23" priority="24">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:C91">
-    <cfRule type="expression" dxfId="24" priority="23">
+    <cfRule type="expression" dxfId="22" priority="23">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:C93">
-    <cfRule type="expression" dxfId="23" priority="22">
+    <cfRule type="expression" dxfId="21" priority="22">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:C95">
-    <cfRule type="expression" dxfId="22" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C96:C97">
-    <cfRule type="expression" dxfId="21" priority="20">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98:C99">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C100:C101">
-    <cfRule type="expression" dxfId="19" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C102:C103">
-    <cfRule type="expression" dxfId="18" priority="17">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104:C105">
-    <cfRule type="expression" dxfId="17" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C106:C107">
-    <cfRule type="expression" dxfId="16" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108:C109">
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C110:C111">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C112:C113">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114:C115">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C116:C117">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C119">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C120:C121">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17509,4 +17608,509 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8816743-55BC-47DB-894C-0BA34DFAD590}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>239</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="E3" s="1">
+        <v>239</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1773</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1773</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>11884</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="E7" s="1">
+        <v>11884</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.999</v>
+      </c>
+      <c r="E8" s="1">
+        <v>56436</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="1">
+        <v>56436</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H2:I9 A2:G3 A4:D4 F4:G4 A5:G9 B10:C15 F10:I15 A10:A30">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>"OR(C:C+I:I=2,C:C+I:I=0)"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>